<commit_message>
19-01-2018 : BugFix : BulkCostCode Upload, FrmBulkSanction
</commit_message>
<xml_diff>
--- a/upload_template/BulkCostCode_Upload.xlsx
+++ b/upload_template/BulkCostCode_Upload.xlsx
@@ -122,7 +122,7 @@
     <t>2017-09-22</t>
   </si>
   <si>
-    <t>CostCode1</t>
+    <t>CostCode</t>
   </si>
 </sst>
 </file>
@@ -460,7 +460,7 @@
   <dimension ref="A1:C214"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>